<commit_message>
fix survey cases, add specialist case
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -5,6 +5,7 @@
   <sheets>
     <sheet state="visible" name="male" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="female" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="specialist" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -12,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1189" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1213" uniqueCount="249">
   <si>
     <t>testCaseName</t>
   </si>
@@ -714,6 +715,51 @@
   </si>
   <si>
     <t>40-45</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Email Address</t>
+  </si>
+  <si>
+    <t>Confirm Email Address</t>
+  </si>
+  <si>
+    <t>STAT patient</t>
+  </si>
+  <si>
+    <t>Type of Cancer-1</t>
+  </si>
+  <si>
+    <t>Age of Diagnosis-1</t>
+  </si>
+  <si>
+    <t>Type of Cancer-2</t>
+  </si>
+  <si>
+    <t>Age of Diagnosis-2</t>
+  </si>
+  <si>
+    <t>specialistE2e-1</t>
+  </si>
+  <si>
+    <t>john</t>
+  </si>
+  <si>
+    <t>doe</t>
+  </si>
+  <si>
+    <t>Chicago - New User Location</t>
+  </si>
+  <si>
+    <t>user@email.com</t>
+  </si>
+  <si>
+    <t>Bladder</t>
+  </si>
+  <si>
+    <t>Adrenal Gland</t>
   </si>
 </sst>
 </file>
@@ -723,7 +769,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm-dd-yyyy"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -744,6 +790,11 @@
       <sz val="9.0"/>
       <color rgb="FF1F1F1F"/>
       <name val="&quot;Google Sans&quot;"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -772,7 +823,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -821,6 +872,12 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf quotePrefix="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -834,6 +891,10 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -4824,4 +4885,101 @@
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>237</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>238</v>
+      </c>
+      <c r="K1" s="16" t="s">
+        <v>239</v>
+      </c>
+      <c r="L1" s="16" t="s">
+        <v>240</v>
+      </c>
+      <c r="M1" s="16" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>243</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>244</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>245</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>246</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>246</v>
+      </c>
+      <c r="I2" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="J2" s="16" t="s">
+        <v>247</v>
+      </c>
+      <c r="K2" s="16">
+        <v>23.0</v>
+      </c>
+      <c r="L2" s="16" t="s">
+        <v>248</v>
+      </c>
+      <c r="M2" s="16">
+        <v>34.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add validation to the specialist case
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1213" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1215" uniqueCount="251">
   <si>
     <t>testCaseName</t>
   </si>
@@ -741,6 +741,9 @@
     <t>Age of Diagnosis-2</t>
   </si>
   <si>
+    <t>eligibilities</t>
+  </si>
+  <si>
     <t>specialistE2e-1</t>
   </si>
   <si>
@@ -760,6 +763,9 @@
   </si>
   <si>
     <t>Adrenal Gland</t>
+  </si>
+  <si>
+    <t>GENETIC TESTING,GENETIC REFERRAL,PROSTATE SCREENING</t>
   </si>
 </sst>
 </file>
@@ -4937,16 +4943,19 @@
       <c r="M1" s="16" t="s">
         <v>241</v>
       </c>
+      <c r="N1" s="16" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D2" s="16" t="s">
         <v>48</v>
@@ -4955,28 +4964,31 @@
         <v>47</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="I2" s="16" t="s">
         <v>49</v>
       </c>
       <c r="J2" s="16" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="K2" s="16">
         <v>23.0</v>
       </c>
       <c r="L2" s="16" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="M2" s="16">
         <v>34.0</v>
+      </c>
+      <c r="N2" s="16" t="s">
+        <v>250</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add test cases for careplan
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -1,19 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\CIQAutomation\src\test\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F3DC28E-709F-4D61-AE12-D23F42C8C900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="male" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="female" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="specialist" sheetId="3" r:id="rId6"/>
+    <sheet name="male" sheetId="1" r:id="rId1"/>
+    <sheet name="female" sheetId="2" r:id="rId2"/>
+    <sheet name="specialist" sheetId="3" r:id="rId3"/>
+    <sheet name="ithaca" sheetId="4" r:id="rId4"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1215" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1348" uniqueCount="329">
   <si>
     <t>testCaseName</t>
   </si>
@@ -766,40 +776,289 @@
   </si>
   <si>
     <t>GENETIC TESTING,GENETIC REFERRAL,PROSTATE SCREENING</t>
+  </si>
+  <si>
+    <t>SpecialistMamogramCheck</t>
+  </si>
+  <si>
+    <t>YJF151102</t>
+  </si>
+  <si>
+    <t>YJL151102</t>
+  </si>
+  <si>
+    <t>Age of Menarche</t>
+  </si>
+  <si>
+    <t>Menopausal Status</t>
+  </si>
+  <si>
+    <t>postmenopausal</t>
+  </si>
+  <si>
+    <t>Number of Breast Biopsies</t>
+  </si>
+  <si>
+    <t>Breast Density</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Number of Colon Polyps</t>
+  </si>
+  <si>
+    <t>ReportName</t>
+  </si>
+  <si>
+    <t>Patient Letter (New)</t>
+  </si>
+  <si>
+    <t>ithacaCarePlanEligibility</t>
+  </si>
+  <si>
+    <t>DayOfBirth</t>
+  </si>
+  <si>
+    <t>MonthOfBirth</t>
+  </si>
+  <si>
+    <t>YearOfBirth</t>
+  </si>
+  <si>
+    <t>Currently Smokes</t>
+  </si>
+  <si>
+    <t>Years Smoked</t>
+  </si>
+  <si>
+    <t>Number of Packs Per Day</t>
+  </si>
+  <si>
+    <t>FEMALE</t>
+  </si>
+  <si>
+    <t>LUNG SCREENING</t>
+  </si>
+  <si>
+    <t>SpecialistAromataseCheck</t>
+  </si>
+  <si>
+    <t>Has Had Genetic Testing</t>
+  </si>
+  <si>
+    <t>Add Pathogenic Mutations1</t>
+  </si>
+  <si>
+    <t>BRCA1</t>
+  </si>
+  <si>
+    <t>Add Pathogenic Mutations2</t>
+  </si>
+  <si>
+    <t>BRCA2</t>
+  </si>
+  <si>
+    <t>Breast ER Status</t>
+  </si>
+  <si>
+    <t>Positive</t>
+  </si>
+  <si>
+    <t>Care Plan</t>
+  </si>
+  <si>
+    <t>Aromatase Inhibitors (Anastrozole 1 mg/day or Exemestane 25mg/d for 5 years) - RECOMMENDED</t>
+  </si>
+  <si>
+    <t>Mammogram (Annual) - RECOMMENDED</t>
+  </si>
+  <si>
+    <t>SpecialistHBOCAndHCCCheck</t>
+  </si>
+  <si>
+    <t>Comorbidity</t>
+  </si>
+  <si>
+    <t>Diabetes Type 2 (CKD)</t>
+  </si>
+  <si>
+    <t>Age of Diagnosis</t>
+  </si>
+  <si>
+    <t>Race</t>
+  </si>
+  <si>
+    <t>Asian</t>
+  </si>
+  <si>
+    <t>Sub Race</t>
+  </si>
+  <si>
+    <t>Japanese</t>
+  </si>
+  <si>
+    <t>Tubal Ligation</t>
+  </si>
+  <si>
+    <t>Surgery</t>
+  </si>
+  <si>
+    <t>premenopausal</t>
+  </si>
+  <si>
+    <t>Gravida</t>
+  </si>
+  <si>
+    <t>Parity</t>
+  </si>
+  <si>
+    <t>Age of First Birth</t>
+  </si>
+  <si>
+    <t>Weight(lb)</t>
+  </si>
+  <si>
+    <t>5 ft 2 in</t>
+  </si>
+  <si>
+    <t>Aunt</t>
+  </si>
+  <si>
+    <t>Maternal</t>
+  </si>
+  <si>
+    <t>Cancer Type1</t>
+  </si>
+  <si>
+    <t>Family Grouping1</t>
+  </si>
+  <si>
+    <t>Age Of Diagnosis1</t>
+  </si>
+  <si>
+    <t>Relationship1</t>
+  </si>
+  <si>
+    <t>Immediate</t>
+  </si>
+  <si>
+    <t>Family Grouping2</t>
+  </si>
+  <si>
+    <t>Age Of Diagnosis2</t>
+  </si>
+  <si>
+    <t>Cancer Type2</t>
+  </si>
+  <si>
+    <t>Relationship2</t>
+  </si>
+  <si>
+    <t>Colorectal</t>
+  </si>
+  <si>
+    <t>Invitae</t>
+  </si>
+  <si>
+    <t>Vendors</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>BRCA 1/2 + Multi-Cancer Panel</t>
+  </si>
+  <si>
+    <t>TestName1</t>
+  </si>
+  <si>
+    <t>TestResultOption1</t>
+  </si>
+  <si>
+    <t>Pathogenic/Deleterious</t>
+  </si>
+  <si>
+    <t>TestName2</t>
+  </si>
+  <si>
+    <t>VUS - Likely Pathogenic</t>
+  </si>
+  <si>
+    <t>TestResultOption2</t>
+  </si>
+  <si>
+    <t>FormNames</t>
+  </si>
+  <si>
+    <t>UHC LMN - HBOC</t>
+  </si>
+  <si>
+    <t>TestName3</t>
+  </si>
+  <si>
+    <t>TestResultOption3</t>
+  </si>
+  <si>
+    <t>ATM</t>
+  </si>
+  <si>
+    <t>VUS - Unknown</t>
+  </si>
+  <si>
+    <t>AdditionalTestResultOption</t>
+  </si>
+  <si>
+    <t>VUS - Likely Benign</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="mm-dd-yyyy"/>
+    <numFmt numFmtId="164" formatCode="mm\-dd\-yyyy"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="9.0"/>
+      <sz val="9"/>
       <color rgb="FF1F1F1F"/>
       <name val="&quot;Google Sans&quot;"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -808,7 +1067,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -824,88 +1083,63 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="14">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf quotePrefix="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf quotePrefix="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf quotePrefix="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf quotePrefix="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -1095,23 +1329,28 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:AR18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="W2" sqref="W2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="11" max="11" width="25.75"/>
+    <col min="11" max="11" width="25.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:44" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1245,7 +1484,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:44" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>44</v>
       </c>
@@ -1379,7 +1618,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:44" ht="15.75" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>72</v>
       </c>
@@ -1513,7 +1752,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:44" ht="15.75" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>79</v>
       </c>
@@ -1647,7 +1886,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:44" ht="15.75" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>84</v>
       </c>
@@ -1781,7 +2020,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:44" ht="15.75" customHeight="1">
       <c r="A6" s="4" t="s">
         <v>90</v>
       </c>
@@ -1873,7 +2112,7 @@
         <v>103</v>
       </c>
       <c r="AG6" s="5">
-        <v>166.0</v>
+        <v>166</v>
       </c>
       <c r="AH6" s="1" t="s">
         <v>49</v>
@@ -1882,24 +2121,24 @@
         <v>49</v>
       </c>
       <c r="AJ6" s="6">
-        <v>40.0</v>
+        <v>40</v>
       </c>
       <c r="AK6" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="AL6" s="7"/>
+      <c r="AL6" s="1"/>
       <c r="AM6" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="AN6" s="7"/>
-      <c r="AO6" s="7"/>
-      <c r="AP6" s="7"/>
+      <c r="AN6" s="1"/>
+      <c r="AO6" s="1"/>
+      <c r="AP6" s="1"/>
       <c r="AQ6" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="AR6" s="7"/>
+      <c r="AR6" s="1"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:44" ht="15.75" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>104</v>
       </c>
@@ -2033,7 +2272,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:44" ht="15.75" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>110</v>
       </c>
@@ -2167,7 +2406,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:44" ht="15.75" customHeight="1">
       <c r="A9" s="4" t="s">
         <v>119</v>
       </c>
@@ -2201,16 +2440,16 @@
       <c r="K9" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="L9" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="M9" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="N9" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="O9" s="8" t="s">
+      <c r="L9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="O9" s="1" t="s">
         <v>52</v>
       </c>
       <c r="P9" s="1" t="s">
@@ -2285,13 +2524,13 @@
       <c r="AM9" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AN9" s="7"/>
-      <c r="AO9" s="7"/>
-      <c r="AP9" s="7"/>
-      <c r="AQ9" s="7"/>
-      <c r="AR9" s="7"/>
+      <c r="AN9" s="1"/>
+      <c r="AO9" s="1"/>
+      <c r="AP9" s="1"/>
+      <c r="AQ9" s="1"/>
+      <c r="AR9" s="1"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:44" ht="15.75" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>123</v>
       </c>
@@ -2325,16 +2564,16 @@
       <c r="K10" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="L10" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="M10" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="N10" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="O10" s="8" t="s">
+      <c r="L10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="O10" s="1" t="s">
         <v>52</v>
       </c>
       <c r="P10" s="1" t="s">
@@ -2425,7 +2664,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:44" ht="15.75" customHeight="1">
       <c r="A11" s="1" t="s">
         <v>128</v>
       </c>
@@ -2532,7 +2771,7 @@
         <v>49</v>
       </c>
       <c r="AJ11" s="6">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="AK11" s="3" t="s">
         <v>132</v>
@@ -2559,7 +2798,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:44" ht="15.75" customHeight="1">
       <c r="A12" s="1" t="s">
         <v>133</v>
       </c>
@@ -2677,9 +2916,9 @@
       <c r="AM12" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="AN12" s="7"/>
-      <c r="AO12" s="7"/>
-      <c r="AP12" s="7"/>
+      <c r="AN12" s="1"/>
+      <c r="AO12" s="1"/>
+      <c r="AP12" s="1"/>
       <c r="AQ12" s="1" t="s">
         <v>49</v>
       </c>
@@ -2687,7 +2926,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:44" ht="15.75" customHeight="1">
       <c r="A13" s="1" t="s">
         <v>137</v>
       </c>
@@ -2794,7 +3033,7 @@
         <v>93</v>
       </c>
       <c r="AJ13" s="6">
-        <v>40.0</v>
+        <v>40</v>
       </c>
       <c r="AK13" s="3" t="s">
         <v>69</v>
@@ -2805,7 +3044,7 @@
       <c r="AM13" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AN13" s="8" t="s">
+      <c r="AN13" s="1" t="s">
         <v>144</v>
       </c>
       <c r="AO13" s="1" t="s">
@@ -2821,7 +3060,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:44" ht="15.75" customHeight="1">
       <c r="A14" s="1" t="s">
         <v>145</v>
       </c>
@@ -2955,28 +3194,29 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15">
-      <c r="D15" s="9"/>
+    <row r="15" spans="1:44" ht="15.75" customHeight="1">
+      <c r="D15" s="7"/>
     </row>
-    <row r="18">
-      <c r="P18" s="10"/>
+    <row r="18" spans="16:16" ht="13.2">
+      <c r="P18" s="8"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:BD14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:56" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3146,14 +3386,14 @@
         <v>171</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:56" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="1" t="s">
         <v>46</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -3270,60 +3510,60 @@
       <c r="AO2" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="AP2" s="8" t="s">
+      <c r="AP2" s="1" t="s">
         <v>185</v>
       </c>
       <c r="AQ2" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="AR2" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="AS2" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="AT2" s="11" t="s">
+      <c r="AR2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AS2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AT2" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="AU2" s="11" t="s">
+      <c r="AU2" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="AV2" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="AW2" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="AX2" s="8" t="s">
+      <c r="AV2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AW2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AX2" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AY2" s="8" t="s">
+      <c r="AY2" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="AZ2" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="BA2" s="8" t="s">
+      <c r="AZ2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="BA2" s="1" t="s">
         <v>49</v>
       </c>
       <c r="BB2" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="BC2" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="BD2" s="8" t="s">
+      <c r="BC2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="BD2" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:56" ht="15.75" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="1" t="s">
         <v>73</v>
       </c>
       <c r="D3" s="3" t="s">
@@ -3440,60 +3680,60 @@
       <c r="AO3" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="AP3" s="8" t="s">
+      <c r="AP3" s="1" t="s">
         <v>185</v>
       </c>
       <c r="AQ3" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="AR3" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="AS3" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="AT3" s="11" t="s">
+      <c r="AR3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AS3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AT3" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="AU3" s="11" t="s">
+      <c r="AU3" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="AV3" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="AW3" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="AX3" s="8" t="s">
+      <c r="AV3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AW3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AX3" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AY3" s="8" t="s">
+      <c r="AY3" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="AZ3" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="BA3" s="8" t="s">
+      <c r="AZ3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="BA3" s="1" t="s">
         <v>49</v>
       </c>
       <c r="BB3" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="BC3" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="BD3" s="8" t="s">
+      <c r="BC3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="BD3" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:56" ht="15.75" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="1" t="s">
         <v>80</v>
       </c>
       <c r="D4" s="3" t="s">
@@ -3571,7 +3811,7 @@
       <c r="AB4" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="AC4" s="12" t="s">
+      <c r="AC4" s="5" t="s">
         <v>197</v>
       </c>
       <c r="AD4" s="1" t="s">
@@ -3589,7 +3829,7 @@
       <c r="AH4" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="AI4" s="11" t="s">
+      <c r="AI4" s="3" t="s">
         <v>199</v>
       </c>
       <c r="AJ4" s="1" t="s">
@@ -3601,69 +3841,69 @@
       <c r="AL4" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="AM4" s="11" t="s">
+      <c r="AM4" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="AN4" s="11" t="s">
+      <c r="AN4" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="AO4" s="11" t="s">
+      <c r="AO4" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="AP4" s="8" t="s">
+      <c r="AP4" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="AQ4" s="11" t="s">
+      <c r="AQ4" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="AR4" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="AS4" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="AT4" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="AU4" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="AV4" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="AW4" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="AX4" s="8" t="s">
+      <c r="AR4" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AS4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AT4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AU4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AV4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AW4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AX4" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="AY4" s="8" t="s">
+      <c r="AY4" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="AZ4" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="BA4" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="BB4" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="BC4" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="BD4" s="8" t="s">
+      <c r="AZ4" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="BA4" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="BB4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="BC4" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="BD4" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:56" ht="15.75" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="1" t="s">
         <v>85</v>
       </c>
       <c r="D5" s="3" t="s">
@@ -3780,60 +4020,60 @@
       <c r="AO5" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="AP5" s="8" t="s">
+      <c r="AP5" s="1" t="s">
         <v>201</v>
       </c>
       <c r="AQ5" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="AR5" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="AS5" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="AT5" s="11" t="s">
+      <c r="AR5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AS5" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AT5" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="AU5" s="11" t="s">
+      <c r="AU5" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="AV5" s="12" t="s">
+      <c r="AV5" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="AW5" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="AX5" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="AY5" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="AZ5" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="BA5" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="BB5" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="BC5" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="BD5" s="8" t="s">
+      <c r="AW5" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AX5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AY5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AZ5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="BA5" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="BB5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="BC5" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="BD5" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:56" ht="15.75" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="1" t="s">
         <v>91</v>
       </c>
       <c r="D6" s="3" t="s">
@@ -3950,60 +4190,60 @@
       <c r="AO6" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="AP6" s="8" t="s">
+      <c r="AP6" s="1" t="s">
         <v>185</v>
       </c>
       <c r="AQ6" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="AR6" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="AS6" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="AT6" s="11" t="s">
+      <c r="AR6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AS6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AT6" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="AU6" s="11" t="s">
+      <c r="AU6" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="AV6" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="AW6" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="AX6" s="8" t="s">
+      <c r="AV6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AW6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AX6" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AY6" s="8" t="s">
+      <c r="AY6" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="AZ6" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="BA6" s="8" t="s">
+      <c r="AZ6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="BA6" s="1" t="s">
         <v>49</v>
       </c>
       <c r="BB6" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="BC6" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="BD6" s="8" t="s">
+      <c r="BC6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="BD6" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:56" ht="15.75" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="1" t="s">
         <v>105</v>
       </c>
       <c r="D7" s="3" t="s">
@@ -4081,7 +4321,7 @@
       <c r="AB7" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="AC7" s="12" t="s">
+      <c r="AC7" s="5" t="s">
         <v>197</v>
       </c>
       <c r="AD7" s="1" t="s">
@@ -4099,7 +4339,7 @@
       <c r="AH7" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="AI7" s="11" t="s">
+      <c r="AI7" s="3" t="s">
         <v>199</v>
       </c>
       <c r="AJ7" s="1" t="s">
@@ -4111,69 +4351,69 @@
       <c r="AL7" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="AM7" s="11" t="s">
+      <c r="AM7" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="AN7" s="11" t="s">
+      <c r="AN7" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="AO7" s="11" t="s">
+      <c r="AO7" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="AP7" s="8" t="s">
+      <c r="AP7" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="AQ7" s="11" t="s">
+      <c r="AQ7" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="AR7" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="AS7" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="AT7" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="AU7" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="AV7" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="AW7" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="AX7" s="8" t="s">
+      <c r="AR7" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AS7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AT7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AU7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AV7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AW7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AX7" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="AY7" s="8" t="s">
+      <c r="AY7" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="AZ7" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="BA7" s="8" t="s">
+      <c r="AZ7" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="BA7" s="1" t="s">
         <v>49</v>
       </c>
       <c r="BB7" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="BC7" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="BD7" s="8" t="s">
+      <c r="BC7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="BD7" s="1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:56" ht="15.75" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="1" t="s">
         <v>111</v>
       </c>
       <c r="D8" s="3" t="s">
@@ -4188,7 +4428,7 @@
       <c r="G8" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="H8" s="1" t="s">
         <v>52</v>
       </c>
       <c r="I8" s="1" t="s">
@@ -4215,7 +4455,7 @@
       <c r="P8" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="Q8" s="8" t="s">
+      <c r="Q8" s="1" t="s">
         <v>52</v>
       </c>
       <c r="R8" s="1" t="s">
@@ -4290,60 +4530,60 @@
       <c r="AO8" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="AP8" s="8" t="s">
+      <c r="AP8" s="1" t="s">
         <v>131</v>
       </c>
       <c r="AQ8" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="AR8" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="AS8" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="AT8" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="AU8" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="AV8" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="AW8" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="AX8" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="AY8" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="AZ8" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="BA8" s="8" t="s">
+      <c r="AR8" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AS8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AT8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AU8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AV8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AW8" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AX8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AY8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AZ8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="BA8" s="1" t="s">
         <v>49</v>
       </c>
       <c r="BB8" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="BC8" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="BD8" s="8" t="s">
+      <c r="BC8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="BD8" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:56" ht="15.75" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="1" t="s">
         <v>120</v>
       </c>
       <c r="D9" s="3" t="s">
@@ -4358,7 +4598,7 @@
       <c r="G9" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="H9" s="8" t="s">
+      <c r="H9" s="1" t="s">
         <v>52</v>
       </c>
       <c r="I9" s="1" t="s">
@@ -4370,13 +4610,13 @@
       <c r="K9" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="L9" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="M9" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="N9" s="8" t="s">
+      <c r="L9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N9" s="1" t="s">
         <v>52</v>
       </c>
       <c r="O9" s="1" t="s">
@@ -4385,7 +4625,7 @@
       <c r="P9" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="Q9" s="8" t="s">
+      <c r="Q9" s="1" t="s">
         <v>52</v>
       </c>
       <c r="R9" s="1" t="s">
@@ -4460,64 +4700,64 @@
       <c r="AO9" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="AP9" s="8" t="s">
+      <c r="AP9" s="1" t="s">
         <v>131</v>
       </c>
       <c r="AQ9" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="AR9" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="AS9" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="AT9" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="AU9" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="AV9" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="AW9" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="AX9" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="AY9" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="AZ9" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="BA9" s="8" t="s">
+      <c r="AR9" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AS9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AT9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AU9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AV9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AW9" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AX9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AY9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AZ9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="BA9" s="1" t="s">
         <v>49</v>
       </c>
       <c r="BB9" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="BC9" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="BD9" s="8" t="s">
+      <c r="BC9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="BD9" s="1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:56" ht="15.75" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="D10" s="13">
-        <v>24691.0</v>
+      <c r="D10" s="9">
+        <v>24691</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>174</v>
@@ -4528,7 +4768,7 @@
       <c r="G10" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="H10" s="8" t="s">
+      <c r="H10" s="1" t="s">
         <v>52</v>
       </c>
       <c r="I10" s="1" t="s">
@@ -4540,13 +4780,13 @@
       <c r="K10" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="L10" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="M10" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="N10" s="8" t="s">
+      <c r="L10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N10" s="1" t="s">
         <v>52</v>
       </c>
       <c r="O10" s="1" t="s">
@@ -4555,7 +4795,7 @@
       <c r="P10" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="Q10" s="8" t="s">
+      <c r="Q10" s="1" t="s">
         <v>52</v>
       </c>
       <c r="R10" s="1" t="s">
@@ -4622,70 +4862,70 @@
         <v>223</v>
       </c>
       <c r="AM10" s="5">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="AN10" s="5">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="AO10" s="5">
-        <v>22.0</v>
-      </c>
-      <c r="AP10" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="AP10" s="1" t="s">
         <v>224</v>
       </c>
       <c r="AQ10" s="5">
-        <v>178.0</v>
-      </c>
-      <c r="AR10" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="AS10" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="AT10" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="AU10" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="AV10" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="AW10" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="AX10" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="AY10" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="AZ10" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="BA10" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="AR10" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AS10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AT10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AU10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AV10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AW10" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AX10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AY10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AZ10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="BA10" s="1" t="s">
         <v>49</v>
       </c>
       <c r="BB10" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="BC10" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="BD10" s="8" t="s">
+      <c r="BC10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="BD10" s="1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:56" ht="15.75" customHeight="1">
       <c r="A11" s="1"/>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="D11" s="13">
-        <v>20308.0</v>
+      <c r="D11" s="9">
+        <v>20308</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>174</v>
@@ -4696,7 +4936,7 @@
       <c r="G11" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="H11" s="8" t="s">
+      <c r="H11" s="1" t="s">
         <v>52</v>
       </c>
       <c r="I11" s="1" t="s">
@@ -4708,68 +4948,68 @@
       <c r="K11" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="L11" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="M11" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="N11" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="O11" s="14"/>
-      <c r="P11" s="7"/>
-      <c r="Q11" s="14"/>
-      <c r="R11" s="14"/>
-      <c r="S11" s="14"/>
-      <c r="T11" s="14"/>
-      <c r="U11" s="14"/>
+      <c r="L11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+      <c r="U11" s="1"/>
       <c r="V11" s="1"/>
-      <c r="W11" s="14"/>
-      <c r="X11" s="14"/>
-      <c r="Y11" s="14"/>
+      <c r="W11" s="1"/>
+      <c r="X11" s="1"/>
+      <c r="Y11" s="1"/>
       <c r="Z11" s="1"/>
-      <c r="AA11" s="14"/>
-      <c r="AB11" s="14"/>
-      <c r="AC11" s="14"/>
+      <c r="AA11" s="1"/>
+      <c r="AB11" s="1"/>
+      <c r="AC11" s="1"/>
       <c r="AD11" s="1"/>
-      <c r="AE11" s="14"/>
-      <c r="AF11" s="14"/>
-      <c r="AG11" s="14"/>
+      <c r="AE11" s="1"/>
+      <c r="AF11" s="1"/>
+      <c r="AG11" s="1"/>
       <c r="AH11" s="1"/>
-      <c r="AI11" s="14"/>
-      <c r="AJ11" s="14"/>
-      <c r="AK11" s="14"/>
-      <c r="AL11" s="14"/>
-      <c r="AM11" s="14"/>
-      <c r="AN11" s="14"/>
-      <c r="AO11" s="14"/>
-      <c r="AP11" s="14"/>
-      <c r="AQ11" s="14"/>
-      <c r="AR11" s="14"/>
-      <c r="AS11" s="14"/>
-      <c r="AT11" s="14"/>
-      <c r="AU11" s="14"/>
-      <c r="AV11" s="14"/>
-      <c r="AW11" s="14"/>
-      <c r="AX11" s="14"/>
-      <c r="AY11" s="14"/>
-      <c r="AZ11" s="14"/>
-      <c r="BA11" s="14"/>
-      <c r="BB11" s="14"/>
-      <c r="BC11" s="14"/>
-      <c r="BD11" s="14"/>
+      <c r="AI11" s="1"/>
+      <c r="AJ11" s="1"/>
+      <c r="AK11" s="1"/>
+      <c r="AL11" s="1"/>
+      <c r="AM11" s="1"/>
+      <c r="AN11" s="1"/>
+      <c r="AO11" s="1"/>
+      <c r="AP11" s="1"/>
+      <c r="AQ11" s="1"/>
+      <c r="AR11" s="1"/>
+      <c r="AS11" s="1"/>
+      <c r="AT11" s="1"/>
+      <c r="AU11" s="1"/>
+      <c r="AV11" s="1"/>
+      <c r="AW11" s="1"/>
+      <c r="AX11" s="1"/>
+      <c r="AY11" s="1"/>
+      <c r="AZ11" s="1"/>
+      <c r="BA11" s="1"/>
+      <c r="BB11" s="1"/>
+      <c r="BC11" s="1"/>
+      <c r="BD11" s="1"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:56" ht="15.75" customHeight="1">
       <c r="A12" s="1"/>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D12" s="15">
-        <v>20308.0</v>
+      <c r="D12" s="9">
+        <v>20308</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>174</v>
@@ -4843,45 +5083,45 @@
         <v>233</v>
       </c>
       <c r="AD12" s="1"/>
-      <c r="AE12" s="7"/>
-      <c r="AF12" s="7"/>
-      <c r="AG12" s="7"/>
+      <c r="AE12" s="1"/>
+      <c r="AF12" s="1"/>
+      <c r="AG12" s="1"/>
       <c r="AH12" s="1"/>
       <c r="AI12" s="5">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="AJ12" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="AK12" s="14"/>
-      <c r="AL12" s="14"/>
-      <c r="AM12" s="14"/>
-      <c r="AN12" s="14"/>
-      <c r="AO12" s="14"/>
-      <c r="AP12" s="14"/>
-      <c r="AQ12" s="14"/>
-      <c r="AR12" s="14"/>
-      <c r="AS12" s="14"/>
-      <c r="AT12" s="14"/>
-      <c r="AU12" s="14"/>
-      <c r="AV12" s="14"/>
-      <c r="AW12" s="14"/>
-      <c r="AX12" s="14"/>
-      <c r="AY12" s="14"/>
-      <c r="AZ12" s="14"/>
-      <c r="BA12" s="14"/>
-      <c r="BB12" s="14"/>
-      <c r="BC12" s="14"/>
-      <c r="BD12" s="14"/>
+      <c r="AK12" s="1"/>
+      <c r="AL12" s="1"/>
+      <c r="AM12" s="1"/>
+      <c r="AN12" s="1"/>
+      <c r="AO12" s="1"/>
+      <c r="AP12" s="1"/>
+      <c r="AQ12" s="1"/>
+      <c r="AR12" s="1"/>
+      <c r="AS12" s="1"/>
+      <c r="AT12" s="1"/>
+      <c r="AU12" s="1"/>
+      <c r="AV12" s="1"/>
+      <c r="AW12" s="1"/>
+      <c r="AX12" s="1"/>
+      <c r="AY12" s="1"/>
+      <c r="AZ12" s="1"/>
+      <c r="BA12" s="1"/>
+      <c r="BB12" s="1"/>
+      <c r="BC12" s="1"/>
+      <c r="BD12" s="1"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:56" ht="15.75" customHeight="1">
       <c r="A13" s="1"/>
       <c r="V13" s="1"/>
       <c r="Z13" s="1"/>
       <c r="AD13" s="1"/>
       <c r="AH13" s="1"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:56" ht="15.75" customHeight="1">
       <c r="A14" s="1"/>
       <c r="V14" s="1"/>
       <c r="Z14" s="1"/>
@@ -4889,21 +5129,27 @@
       <c r="AH14" s="1"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:BB5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="AP1" workbookViewId="0">
+      <selection activeCell="AX16" sqref="AX16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
+  <cols>
+    <col min="39" max="39" width="16.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:54" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4919,79 +5165,566 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="10" t="s">
         <v>234</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="10" t="s">
         <v>235</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="10" t="s">
         <v>236</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="10" t="s">
         <v>237</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="J1" s="10" t="s">
         <v>238</v>
       </c>
-      <c r="K1" s="16" t="s">
+      <c r="K1" s="10" t="s">
         <v>239</v>
       </c>
-      <c r="L1" s="16" t="s">
+      <c r="L1" s="10" t="s">
         <v>240</v>
       </c>
-      <c r="M1" s="16" t="s">
+      <c r="M1" s="10" t="s">
         <v>241</v>
       </c>
-      <c r="N1" s="16" t="s">
+      <c r="N1" s="10" t="s">
         <v>242</v>
       </c>
+      <c r="O1" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="P1" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="Q1" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="R1" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="S1" s="10" t="s">
+        <v>260</v>
+      </c>
+      <c r="T1" s="10" t="s">
+        <v>261</v>
+      </c>
+      <c r="U1" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="V1" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="W1" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="X1" s="10" t="s">
+        <v>278</v>
+      </c>
+      <c r="Y1" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="Z1" s="10" t="s">
+        <v>284</v>
+      </c>
+      <c r="AA1" s="10" t="s">
+        <v>286</v>
+      </c>
+      <c r="AB1" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="AC1" s="10" t="s">
+        <v>289</v>
+      </c>
+      <c r="AD1" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="AE1" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="AF1" s="10" t="s">
+        <v>295</v>
+      </c>
+      <c r="AG1" s="10" t="s">
+        <v>296</v>
+      </c>
+      <c r="AH1" s="10" t="s">
+        <v>297</v>
+      </c>
+      <c r="AI1" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AJ1" s="10" t="s">
+        <v>312</v>
+      </c>
+      <c r="AK1" s="10" t="s">
+        <v>313</v>
+      </c>
+      <c r="AL1" s="10" t="s">
+        <v>315</v>
+      </c>
+      <c r="AM1" s="10" t="s">
+        <v>316</v>
+      </c>
+      <c r="AN1" s="10" t="s">
+        <v>318</v>
+      </c>
+      <c r="AO1" s="10" t="s">
+        <v>320</v>
+      </c>
+      <c r="AP1" s="10" t="s">
+        <v>321</v>
+      </c>
+      <c r="AQ1" s="10" t="s">
+        <v>323</v>
+      </c>
+      <c r="AR1" s="10" t="s">
+        <v>324</v>
+      </c>
+      <c r="AS1" s="10" t="s">
+        <v>327</v>
+      </c>
+      <c r="AT1" s="10" t="s">
+        <v>302</v>
+      </c>
+      <c r="AU1" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="AV1" s="10" t="s">
+        <v>301</v>
+      </c>
+      <c r="AW1" s="10" t="s">
+        <v>302</v>
+      </c>
+      <c r="AX1" s="10" t="s">
+        <v>303</v>
+      </c>
+      <c r="AY1" s="10" t="s">
+        <v>309</v>
+      </c>
+      <c r="AZ1" s="10" t="s">
+        <v>308</v>
+      </c>
+      <c r="BA1" s="10" t="s">
+        <v>306</v>
+      </c>
+      <c r="BB1" s="10" t="s">
+        <v>307</v>
+      </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:54" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="10" t="s">
         <v>245</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="10" t="s">
         <v>246</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="10" t="s">
         <v>247</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="H2" s="10" t="s">
         <v>247</v>
       </c>
-      <c r="I2" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="J2" s="16" t="s">
+      <c r="I2" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="J2" s="10" t="s">
         <v>248</v>
       </c>
-      <c r="K2" s="16">
-        <v>23.0</v>
-      </c>
-      <c r="L2" s="16" t="s">
+      <c r="K2" s="10">
+        <v>23</v>
+      </c>
+      <c r="L2" s="10" t="s">
         <v>249</v>
       </c>
-      <c r="M2" s="16">
-        <v>34.0</v>
-      </c>
-      <c r="N2" s="16" t="s">
+      <c r="M2" s="10">
+        <v>34</v>
+      </c>
+      <c r="N2" s="13" t="s">
         <v>250</v>
+      </c>
+    </row>
+    <row r="3" spans="1:54" ht="15.75" customHeight="1">
+      <c r="A3" t="s">
+        <v>251</v>
+      </c>
+      <c r="B3" t="s">
+        <v>252</v>
+      </c>
+      <c r="C3" t="s">
+        <v>253</v>
+      </c>
+      <c r="D3" t="s">
+        <v>174</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="O3">
+        <v>11</v>
+      </c>
+      <c r="P3" t="s">
+        <v>256</v>
+      </c>
+      <c r="Q3">
+        <v>2</v>
+      </c>
+      <c r="R3" t="s">
+        <v>259</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3" t="s">
+        <v>262</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="4" spans="1:54" ht="15.75" customHeight="1">
+      <c r="A4" t="s">
+        <v>272</v>
+      </c>
+      <c r="B4" t="s">
+        <v>252</v>
+      </c>
+      <c r="C4" t="s">
+        <v>253</v>
+      </c>
+      <c r="D4" t="s">
+        <v>174</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="O4">
+        <v>11</v>
+      </c>
+      <c r="P4" t="s">
+        <v>256</v>
+      </c>
+      <c r="Q4">
+        <v>2</v>
+      </c>
+      <c r="R4" t="s">
+        <v>259</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4" t="s">
+        <v>262</v>
+      </c>
+      <c r="U4" t="s">
+        <v>49</v>
+      </c>
+      <c r="V4" t="s">
+        <v>275</v>
+      </c>
+      <c r="W4" t="s">
+        <v>277</v>
+      </c>
+      <c r="X4" t="s">
+        <v>279</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="5" spans="1:54" ht="15.75" customHeight="1">
+      <c r="A5" t="s">
+        <v>283</v>
+      </c>
+      <c r="C5" t="s">
+        <v>253</v>
+      </c>
+      <c r="D5" t="s">
+        <v>174</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="P5" t="s">
+        <v>293</v>
+      </c>
+      <c r="U5" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>285</v>
+      </c>
+      <c r="AA5">
+        <v>39</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>288</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>290</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>291</v>
+      </c>
+      <c r="AE5">
+        <v>1</v>
+      </c>
+      <c r="AF5">
+        <v>1</v>
+      </c>
+      <c r="AG5">
+        <v>25</v>
+      </c>
+      <c r="AH5">
+        <v>178</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>298</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>311</v>
+      </c>
+      <c r="AK5" t="s">
+        <v>314</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>275</v>
+      </c>
+      <c r="AM5" t="s">
+        <v>317</v>
+      </c>
+      <c r="AN5" t="s">
+        <v>277</v>
+      </c>
+      <c r="AO5" t="s">
+        <v>319</v>
+      </c>
+      <c r="AP5" t="s">
+        <v>322</v>
+      </c>
+      <c r="AQ5" t="s">
+        <v>325</v>
+      </c>
+      <c r="AR5" t="s">
+        <v>326</v>
+      </c>
+      <c r="AS5" t="s">
+        <v>328</v>
+      </c>
+      <c r="AT5" s="10" t="s">
+        <v>300</v>
+      </c>
+      <c r="AU5" s="10" t="s">
+        <v>299</v>
+      </c>
+      <c r="AV5" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="AW5" s="10" t="s">
+        <v>300</v>
+      </c>
+      <c r="AX5">
+        <v>45</v>
+      </c>
+      <c r="AY5" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="AZ5" s="10" t="s">
+        <v>310</v>
+      </c>
+      <c r="BA5" t="s">
+        <v>305</v>
+      </c>
+      <c r="BB5">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EC8B2C0-C7A8-4BB9-8DC4-370C5DC7310E}">
+  <dimension ref="A1:T2"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:S2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetData>
+    <row r="1" spans="1:20" ht="15.75" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>265</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>266</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>267</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>268</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>269</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>301</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>302</v>
+      </c>
+      <c r="O1" s="10" t="s">
+        <v>303</v>
+      </c>
+      <c r="P1" s="10" t="s">
+        <v>309</v>
+      </c>
+      <c r="Q1" s="10" t="s">
+        <v>308</v>
+      </c>
+      <c r="R1" s="10" t="s">
+        <v>306</v>
+      </c>
+      <c r="S1" s="10" t="s">
+        <v>307</v>
+      </c>
+      <c r="T1" s="10"/>
+    </row>
+    <row r="2" spans="1:20" ht="15.75" customHeight="1">
+      <c r="A2" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>244</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>270</v>
+      </c>
+      <c r="E2" s="11">
+        <v>12</v>
+      </c>
+      <c r="F2" s="10">
+        <v>12</v>
+      </c>
+      <c r="G2" s="10">
+        <v>1970</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="I2" s="10">
+        <v>11</v>
+      </c>
+      <c r="J2" s="10">
+        <v>2</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>271</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>299</v>
+      </c>
+      <c r="M2" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="N2" s="10" t="s">
+        <v>300</v>
+      </c>
+      <c r="O2">
+        <v>45</v>
+      </c>
+      <c r="P2" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q2" s="10" t="s">
+        <v>310</v>
+      </c>
+      <c r="R2" t="s">
+        <v>305</v>
+      </c>
+      <c r="S2">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add delphi navigation (#2)
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -1,29 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CIQ-Workspace\CIQAutomation\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF8AC5F1-0DC5-4BFB-A947-B79F6360FE4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABC80B87-3EB5-4CF2-B0B4-A4FAE495BDF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="male" sheetId="1" r:id="rId1"/>
     <sheet name="female" sheetId="2" r:id="rId2"/>
     <sheet name="specialist" sheetId="3" r:id="rId3"/>
-    <sheet name="ithaca" sheetId="4" r:id="rId4"/>
+    <sheet name="delphi" sheetId="5" r:id="rId4"/>
+    <sheet name="ithaca" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1472" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1500" uniqueCount="411">
   <si>
     <t>testCaseName</t>
   </si>
@@ -1181,6 +1182,81 @@
   </si>
   <si>
     <t>readReports</t>
+  </si>
+  <si>
+    <t>delphiNavigation</t>
+  </si>
+  <si>
+    <t>HeaderName</t>
+  </si>
+  <si>
+    <t>Site Administration</t>
+  </si>
+  <si>
+    <t>Dashboard</t>
+  </si>
+  <si>
+    <t>DashboardField</t>
+  </si>
+  <si>
+    <t>DashboardLink</t>
+  </si>
+  <si>
+    <t>Applications</t>
+  </si>
+  <si>
+    <t>LinkName1</t>
+  </si>
+  <si>
+    <t>Location themes</t>
+  </si>
+  <si>
+    <t>Questions</t>
+  </si>
+  <si>
+    <t>Surveys</t>
+  </si>
+  <si>
+    <t>Survey modules</t>
+  </si>
+  <si>
+    <t>LinkName2</t>
+  </si>
+  <si>
+    <t>LinkName3</t>
+  </si>
+  <si>
+    <t>LinkName4</t>
+  </si>
+  <si>
+    <t>LinkName5</t>
+  </si>
+  <si>
+    <t>ApplicationsearchText</t>
+  </si>
+  <si>
+    <t>Family</t>
+  </si>
+  <si>
+    <t>location test</t>
+  </si>
+  <si>
+    <t>Location data test</t>
+  </si>
+  <si>
+    <t>LocationText</t>
+  </si>
+  <si>
+    <t>DataText</t>
+  </si>
+  <si>
+    <t>SurveyModuleText</t>
+  </si>
+  <si>
+    <t>Survey</t>
+  </si>
+  <si>
+    <t>QuestionText</t>
   </si>
 </sst>
 </file>
@@ -5318,8 +5394,8 @@
   </sheetPr>
   <dimension ref="A1:CC9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -6208,6 +6284,115 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3729007F-8007-454B-AE2E-9C2D554BF2E3}">
+  <dimension ref="A1:N2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P11" sqref="P11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2"/>
+  <cols>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+    <col min="3" max="3" width="16.88671875" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="15.6">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" t="s">
+        <v>386</v>
+      </c>
+      <c r="B2" t="s">
+        <v>388</v>
+      </c>
+      <c r="C2" t="s">
+        <v>389</v>
+      </c>
+      <c r="D2" t="s">
+        <v>389</v>
+      </c>
+      <c r="E2" t="s">
+        <v>392</v>
+      </c>
+      <c r="F2" t="s">
+        <v>394</v>
+      </c>
+      <c r="G2" t="s">
+        <v>395</v>
+      </c>
+      <c r="H2" t="s">
+        <v>396</v>
+      </c>
+      <c r="I2" t="s">
+        <v>397</v>
+      </c>
+      <c r="J2" t="s">
+        <v>403</v>
+      </c>
+      <c r="K2" t="s">
+        <v>404</v>
+      </c>
+      <c r="L2" t="s">
+        <v>405</v>
+      </c>
+      <c r="M2" t="s">
+        <v>409</v>
+      </c>
+      <c r="N2" t="s">
+        <v>409</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EC8B2C0-C7A8-4BB9-8DC4-370C5DC7310E}">
   <dimension ref="A1:T2"/>
   <sheetViews>

</xml_diff>

<commit_message>
add american survey test
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -8,23 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CIQ-Workspace\CIQAutomation\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF9B60BF-796E-427F-911D-075E62F4E9E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6565D88E-60C1-4FCC-B846-2094B1715E99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="male" sheetId="1" r:id="rId1"/>
-    <sheet name="female" sheetId="2" r:id="rId2"/>
-    <sheet name="specialist" sheetId="3" r:id="rId3"/>
-    <sheet name="delphi" sheetId="5" r:id="rId4"/>
-    <sheet name="ithaca" sheetId="4" r:id="rId5"/>
+    <sheet name="americansurvey" sheetId="6" r:id="rId2"/>
+    <sheet name="female" sheetId="2" r:id="rId3"/>
+    <sheet name="specialist" sheetId="3" r:id="rId4"/>
+    <sheet name="delphi" sheetId="5" r:id="rId5"/>
+    <sheet name="ithaca" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1759" uniqueCount="414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2361" uniqueCount="417">
   <si>
     <t>testCaseName</t>
   </si>
@@ -1266,6 +1267,15 @@
   </si>
   <si>
     <t>Buccal Swab</t>
+  </si>
+  <si>
+    <t>Had genetic test for hereditary cancer syndromes</t>
+  </si>
+  <si>
+    <t>Tested positive for lynch syndrome</t>
+  </si>
+  <si>
+    <t>Tested positive for BRCA1 or BRCA2</t>
   </si>
 </sst>
 </file>
@@ -1604,8 +1614,8 @@
   </sheetPr>
   <dimension ref="A1:AR18"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="W2" sqref="W2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -3469,6 +3479,1893 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1493E2CB-7966-432A-9ABC-233E6059D6D0}">
+  <dimension ref="A1:AU18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
+  <cols>
+    <col min="11" max="11" width="25.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:47" ht="15.75" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="2" spans="1:47" ht="15.75" customHeight="1">
+      <c r="A2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AG2" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AJ2" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AK2" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AL2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AM2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AN2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AO2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AP2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AQ2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AR2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AS2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AT2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AU2" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:47" ht="15.75" customHeight="1">
+      <c r="A3" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF3" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AG3" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AI3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AJ3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AK3" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AL3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AM3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AN3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AO3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AP3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AQ3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AR3" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:47" ht="15.75" customHeight="1">
+      <c r="A4" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF4" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG4" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AI4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AJ4" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AK4" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AL4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AM4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AN4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AO4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AP4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AQ4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AR4" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:47" ht="15.75" customHeight="1">
+      <c r="A5" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB5" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD5" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE5" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF5" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG5" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="AH5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AI5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AJ5" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AK5" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AL5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AM5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AN5" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AO5" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AP5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AQ5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AR5" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:47" ht="15.75" customHeight="1">
+      <c r="A6" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="W6" s="1"/>
+      <c r="X6" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z6" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AA6" s="1"/>
+      <c r="AB6" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AC6" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AD6" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AE6" s="1"/>
+      <c r="AF6" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AG6" s="5">
+        <v>166</v>
+      </c>
+      <c r="AH6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AI6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AJ6" s="6">
+        <v>40</v>
+      </c>
+      <c r="AK6" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AL6" s="1"/>
+      <c r="AM6" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AN6" s="1"/>
+      <c r="AO6" s="1"/>
+      <c r="AP6" s="1"/>
+      <c r="AQ6" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AR6" s="1"/>
+    </row>
+    <row r="7" spans="1:47" ht="15.75" customHeight="1">
+      <c r="A7" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AF7" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG7" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AH7" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AI7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AJ7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AK7" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AL7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AM7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AN7" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="AO7" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="AP7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AQ7" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AR7" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:47" ht="15.75" customHeight="1">
+      <c r="A8" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="X8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AF8" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AG8" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AH8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AI8" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AJ8" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="AK8" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AL8" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="AM8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AN8" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AO8" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="AP8" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AQ8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AR8" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:47" ht="15.75" customHeight="1">
+      <c r="A9" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="U9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="X9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AF9" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AG9" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AH9" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AI9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AJ9" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="AK9" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AL9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AM9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AN9" s="1"/>
+      <c r="AO9" s="1"/>
+      <c r="AP9" s="1"/>
+      <c r="AQ9" s="1"/>
+      <c r="AR9" s="1"/>
+    </row>
+    <row r="10" spans="1:47" ht="15.75" customHeight="1">
+      <c r="A10" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="U10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="V10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="W10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="X10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AF10" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AG10" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AH10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AI10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AJ10" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="AK10" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AL10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AM10" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AN10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AO10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AP10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AQ10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AR10" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="11" spans="1:47" ht="15.75" customHeight="1">
+      <c r="A11" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="T11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="U11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="V11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="W11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="X11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AF11" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="AG11" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AH11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AI11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AJ11" s="6">
+        <v>25</v>
+      </c>
+      <c r="AK11" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="AL11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AM11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AN11" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AO11" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AP11" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="AQ11" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AR11" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:47" ht="15.75" customHeight="1">
+      <c r="A12" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="S12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="T12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="U12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="V12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="W12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="X12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AF12" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="AG12" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AH12" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AI12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AJ12" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="AK12" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AL12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AM12" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AN12" s="1"/>
+      <c r="AO12" s="1"/>
+      <c r="AP12" s="1"/>
+      <c r="AQ12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AR12" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13" spans="1:47" ht="15.75" customHeight="1">
+      <c r="A13" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="R13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="S13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="T13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="U13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="V13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="W13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="X13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AF13" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="AG13" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="AH13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AI13" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AJ13" s="6">
+        <v>40</v>
+      </c>
+      <c r="AK13" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AL13" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="AM13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AN13" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="AO13" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AP13" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AQ13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AR13" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:47" ht="15.75" customHeight="1">
+      <c r="A14" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="R14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="S14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="T14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="U14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="V14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="W14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="X14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AF14" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG14" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="AH14" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AI14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AJ14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AK14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AL14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AM14" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AN14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AO14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AP14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AQ14" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AR14" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:47" ht="15.75" customHeight="1">
+      <c r="D15" s="7"/>
+    </row>
+    <row r="18" spans="16:16" ht="13.2">
+      <c r="P18" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -5396,14 +7293,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:CE14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AX1" workbookViewId="0">
+    <sheetView topLeftCell="AX1" workbookViewId="0">
       <selection activeCell="BG14" sqref="BG14"/>
     </sheetView>
   </sheetViews>
@@ -7254,7 +9151,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3729007F-8007-454B-AE2E-9C2D554BF2E3}">
   <dimension ref="A1:N2"/>
   <sheetViews>
@@ -7363,7 +9260,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EC8B2C0-C7A8-4BB9-8DC4-370C5DC7310E}">
   <dimension ref="A1:T2"/>
   <sheetViews>

</xml_diff>